<commit_message>
Consumption Schedule Epic and Selenium Method
</commit_message>
<xml_diff>
--- a/src/test/resources/data/SalesforceData.xlsx
+++ b/src/test/resources/data/SalesforceData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Testing\TestLeaf\Eclispe Workspaces\Automation\MavenProject\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C5D1CC-E266-4F75-8CFA-FE3C130235EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95059679-8A03-4B5E-8BF0-8DC40FAF57AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,31 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Sunil</t>
-  </si>
-  <si>
-    <t>Kumar</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Unique ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>TestDataID</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>mercury.bootcamp@testleaf.com</t>
+  </si>
+  <si>
+    <t>Bootcamp@123</t>
+  </si>
+  <si>
+    <t>TD001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,13 +83,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -357,50 +371,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0AF647E1-2267-4C5D-B798-A7431833E01E}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{A6481A62-D86C-4421-B8D8-1C485ABC7794}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>